<commit_message>
2024.09.30 LeetCodeHot100 二刷 每日打卡更新
</commit_message>
<xml_diff>
--- a/2024 每日打卡.xlsx
+++ b/2024 每日打卡.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B89000-F948-4D52-BB10-DAC4CAF68FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8758223-0048-48E3-9A8E-E3494D22357D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9" yWindow="9" windowWidth="21925" windowHeight="11605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="181">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -603,6 +603,115 @@
   </si>
   <si>
     <t>俯卧撑50 蹬车180</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.09.24</t>
+  </si>
+  <si>
+    <t>2024.09.25</t>
+  </si>
+  <si>
+    <t>2024.09.26</t>
+  </si>
+  <si>
+    <t>2024.09.27</t>
+  </si>
+  <si>
+    <t>2024.09.28</t>
+  </si>
+  <si>
+    <t>2024.09.29</t>
+  </si>
+  <si>
+    <t>2024.09.30</t>
+  </si>
+  <si>
+    <t>08:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02:23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23:58</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>秋山梨、水蜜桃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俯卧撑60 蹬车200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俯卧撑34 蹬车230</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俯卧撑60 蹬车220</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香蕉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火龙果、芒果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俯卧撑60 蹬车250</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俯卧撑50 蹬车230</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.10.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尝新 梅一岐山臊子面</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1068,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1819,7 +1928,7 @@
       </c>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>106</v>
       </c>
@@ -1841,7 +1950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -1867,7 +1976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>133</v>
       </c>
@@ -1891,7 +2000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>134</v>
       </c>
@@ -1913,7 +2022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>135</v>
       </c>
@@ -1935,7 +2044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>136</v>
       </c>
@@ -1957,15 +2066,219 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>137</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>142</v>
       </c>
+      <c r="C39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>148</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="11"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024.10.08 LeetCodeHot100 二刷 每日打卡更新
</commit_message>
<xml_diff>
--- a/2024 每日打卡.xlsx
+++ b/2024 每日打卡.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8758223-0048-48E3-9A8E-E3494D22357D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D9371C-13E5-44FD-B630-863EF8DCB1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9" yWindow="9" windowWidth="21925" windowHeight="11605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="214">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -712,6 +712,132 @@
   </si>
   <si>
     <t>尝新 梅一岐山臊子面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.10.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.10.03</t>
+  </si>
+  <si>
+    <t>2024.10.04</t>
+  </si>
+  <si>
+    <t>2024.10.05</t>
+  </si>
+  <si>
+    <t>2024.10.06</t>
+  </si>
+  <si>
+    <t>2024.10.07</t>
+  </si>
+  <si>
+    <t>03:14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23:35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23:42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09:18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09:39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01:42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23:07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>05:19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.10.08</t>
+  </si>
+  <si>
+    <t>爸爸 西津渡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>焦山 朱光玉火锅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>居家休息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爷爷奶奶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冠城 浴火之路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高邮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>南京</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俯卧撑30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俯卧撑20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>梨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香瓜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1177,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2261,6 +2387,9 @@
       <c r="E46" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="G46" s="8" t="s">
+        <v>187</v>
+      </c>
       <c r="H46" s="1" t="s">
         <v>8</v>
       </c>
@@ -2280,6 +2409,196 @@
       <c r="A48" s="5" t="s">
         <v>179</v>
       </c>
+      <c r="B48" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>